<commit_message>
nunit, Customer, DataProvider, pageFactory added.LoginPage Builder refactored.
nunit, Customer, DataProvider, pageFactory added.LoginPage Builder refactored.
</commit_message>
<xml_diff>
--- a/WEVDRIVER_NOTES.xlsx
+++ b/WEVDRIVER_NOTES.xlsx
@@ -4,23 +4,24 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="5" r:id="rId1"/>
     <sheet name="ISSUES" sheetId="6" r:id="rId2"/>
     <sheet name="Notes" sheetId="7" r:id="rId3"/>
-    <sheet name="Chrome" sheetId="1" r:id="rId4"/>
-    <sheet name="Firefox" sheetId="2" r:id="rId5"/>
-    <sheet name="IE" sheetId="3" r:id="rId6"/>
-    <sheet name="EDGE" sheetId="4" r:id="rId7"/>
+    <sheet name="Framework" sheetId="8" r:id="rId4"/>
+    <sheet name="Chrome" sheetId="1" r:id="rId5"/>
+    <sheet name="Firefox" sheetId="2" r:id="rId6"/>
+    <sheet name="IE" sheetId="3" r:id="rId7"/>
+    <sheet name="EDGE" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>https://automatetheplanet.com/advanced-webdriver-tips-tricks-part-1/</t>
   </si>
@@ -420,6 +421,9 @@
       </rPr>
       <t>(driver).MoveToElement(loginName); doesn't work in FF</t>
     </r>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/38956452/c-sharp-extending-selenium-webdriver-class</t>
   </si>
 </sst>
 </file>
@@ -566,8 +570,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -583,9 +587,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -623,7 +627,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -695,7 +699,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1175,7 +1179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1265,6 +1269,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="87.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
@@ -1275,7 +1302,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1287,7 +1314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1301,7 +1328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>